<commit_message>
import customer and supplier
</commit_message>
<xml_diff>
--- a/gkwebapp/static/spreadsheets/Customer_Supplier_Sample_Spreadsheet.xlsx
+++ b/gkwebapp/static/spreadsheets/Customer_Supplier_Sample_Spreadsheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -50,6 +50,33 @@
     <t xml:space="preserve">GSTIN</t>
   </si>
   <si>
+    <t xml:space="preserve">Customer A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. road, Andheri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maharashtra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABWEE8934A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27ABWEE8934A2Z9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23ABCSE1234A2Z3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goa</t>
+  </si>
+  <si>
     <t xml:space="preserve">Account Number</t>
   </si>
   <si>
@@ -60,6 +87,33 @@
   </si>
   <si>
     <t xml:space="preserve">IFSC Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEH, Andheri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIDC, Andheri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCDE8934A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30ABCDE8934A2Z9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andheri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBI00123</t>
   </si>
 </sst>
 </file>
@@ -69,7 +123,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -90,6 +144,18 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,19 +200,27 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -156,10 +230,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -196,7 +270,58 @@
         <v>8</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>9876543210</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>423031</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>987645</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>233445</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="sample@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -212,10 +337,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -252,19 +377,86 @@
         <v>8</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="K1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>323363</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>9120456751</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>9876543210</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>12</v>
+      <c r="D3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>455667</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>9120456752</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>9800765432</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I4" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="sample@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>